<commit_message>
Completed matrix multiplication of CAT across all years; minor correction made to synonym file
</commit_message>
<xml_diff>
--- a/Data/PreprocessedData/MasterSynonymCorrections.xlsx
+++ b/Data/PreprocessedData/MasterSynonymCorrections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19005" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19005" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSynonymCorrections" sheetId="1" r:id="rId1"/>
@@ -3676,9 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D685"/>
   <sheetViews>
-    <sheetView topLeftCell="A659" workbookViewId="0">
-      <selection activeCell="C659" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7451,7 +7449,7 @@
         <v>329</v>
       </c>
       <c r="D269" t="s">
-        <v>101</v>
+        <v>339</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -13483,7 +13481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+    <sheetView topLeftCell="A129" workbookViewId="0">
       <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>

</xml_diff>